<commit_message>
Changed format in several Excel files. Adjusted portfolios classification chart
</commit_message>
<xml_diff>
--- a/DJ30_data_1.xlsx
+++ b/DJ30_data_1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanessa.serrano\Desktop\IQS(2020-21)\ASISTEMBE\ProjecteFinanceStudents\AnalysisR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordi2021\Recerca_Articles\2022Pre_Financial\EventStudies4Finance-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818CECC-84DC-4110-B2EF-E9A056B71413}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA556AF-6B48-4537-8AEE-0A1E29129727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{3D739962-FA6D-48D4-8191-9E4C06016CDA}"/>
+    <workbookView xWindow="20400" yWindow="45" windowWidth="28890" windowHeight="9825" xr2:uid="{3D739962-FA6D-48D4-8191-9E4C06016CDA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -604,7 +604,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>